<commit_message>
v4.0 add log leve warning
</commit_message>
<xml_diff>
--- a/20200506 linux log troubleshooting 特征V4.0.xlsx
+++ b/20200506 linux log troubleshooting 特征V4.0.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="100">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -180,19 +181,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>warn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>VFS  *** too many</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Refuse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>error</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -348,11 +341,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/var/log/mysql/error.log
-systemctl status mysql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>./nginx/logs/error.log</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -395,35 +383,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>xenserver</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/var/log/xhad.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>err</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>timeout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/var/log/xhad.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kvm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ceph</t>
+    <t>fatal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>warn | timeout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日志登记（0-7标准）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>errors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>critical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>critical 马上要处理关注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>errors 留意，回头分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交版本内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加危急故障登记 红色立即处理；黄色留意</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zengxl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zengxl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -431,7 +431,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +456,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
@@ -514,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,6 +550,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -847,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57:E58"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -858,13 +869,14 @@
     <col min="1" max="1" width="21.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="30.75" style="2" customWidth="1"/>
-    <col min="7" max="7" width="58.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="30.75" style="2" customWidth="1"/>
+    <col min="8" max="8" width="58.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -875,19 +887,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -895,20 +910,23 @@
         <v>7</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
+      <c r="D2" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -916,20 +934,23 @@
         <v>7</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -937,18 +958,21 @@
         <v>7</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -956,18 +980,21 @@
         <v>11</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -975,18 +1002,23 @@
         <v>11</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -994,18 +1026,23 @@
         <v>11</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1013,18 +1050,21 @@
         <v>11</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1032,18 +1072,21 @@
         <v>11</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1051,18 +1094,21 @@
         <v>11</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="F10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1070,18 +1116,21 @@
         <v>24</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1089,18 +1138,21 @@
         <v>24</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1108,18 +1160,21 @@
         <v>24</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1127,18 +1182,21 @@
         <v>24</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1146,18 +1204,21 @@
         <v>24</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1165,18 +1226,21 @@
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="F16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1184,18 +1248,21 @@
       <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="F17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1203,18 +1270,21 @@
       <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="F18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1222,18 +1292,21 @@
       <c r="C19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="F19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1241,18 +1314,21 @@
       <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1260,18 +1336,21 @@
       <c r="C21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="F21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1279,16 +1358,19 @@
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="1"/>
+      <c r="D22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1296,16 +1378,19 @@
       <c r="C23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" s="1"/>
+      <c r="D23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1313,17 +1398,20 @@
       <c r="C24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="D24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1331,20 +1419,21 @@
         <v>24</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F25" s="7" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1352,18 +1441,21 @@
         <v>24</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
-        <v>45</v>
+      <c r="D26" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1371,18 +1463,21 @@
         <v>24</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
-        <v>45</v>
+      <c r="D27" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1390,18 +1485,21 @@
         <v>24</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="1" t="s">
-        <v>46</v>
+      <c r="D28" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1409,18 +1507,21 @@
         <v>24</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="1" t="s">
-        <v>46</v>
+      <c r="D29" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1428,18 +1529,21 @@
         <v>24</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="1" t="s">
-        <v>46</v>
+      <c r="D30" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1447,18 +1551,21 @@
         <v>24</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="D31" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1467,17 +1574,20 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1485,18 +1595,21 @@
         <v>24</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F33" s="1" t="s">
+      <c r="D33" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1504,20 +1617,23 @@
         <v>24</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1525,18 +1641,21 @@
         <v>24</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="1" t="s">
-        <v>60</v>
+      <c r="D35" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1544,18 +1663,21 @@
         <v>24</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>60</v>
+      <c r="D36" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1563,18 +1685,21 @@
         <v>24</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>60</v>
+      <c r="D37" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1582,20 +1707,21 @@
         <v>24</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>89</v>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1603,20 +1729,21 @@
         <v>24</v>
       </c>
       <c r="C39" s="7"/>
-      <c r="D39" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>89</v>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1624,20 +1751,21 @@
         <v>24</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>89</v>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1645,20 +1773,21 @@
         <v>24</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>89</v>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1666,20 +1795,21 @@
         <v>24</v>
       </c>
       <c r="C42" s="7"/>
-      <c r="D42" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>89</v>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1687,20 +1817,21 @@
         <v>24</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>89</v>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1708,20 +1839,21 @@
         <v>24</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>89</v>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1729,20 +1861,21 @@
         <v>24</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="D45" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>89</v>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1750,20 +1883,21 @@
         <v>24</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>89</v>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1771,20 +1905,21 @@
         <v>24</v>
       </c>
       <c r="C47" s="7"/>
-      <c r="D47" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>89</v>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1792,20 +1927,21 @@
         <v>24</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>89</v>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1813,20 +1949,21 @@
         <v>24</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="D49" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>89</v>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1834,20 +1971,21 @@
         <v>24</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>89</v>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1855,20 +1993,21 @@
         <v>24</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>89</v>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1876,20 +2015,21 @@
         <v>24</v>
       </c>
       <c r="C52" s="7"/>
-      <c r="D52" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>89</v>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1897,115 +2037,125 @@
         <v>24</v>
       </c>
       <c r="C53" s="7"/>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="7"/>
+      <c r="E53" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F53" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E53" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>89</v>
-      </c>
       <c r="G53" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>53</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
-        <v>54</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
-        <v>56</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>57</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>58</v>
-      </c>
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>59</v>
-      </c>
+      <c r="H59" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="11">
+        <v>43960</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="11">
+        <v>43962</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v4.0 check the log level
</commit_message>
<xml_diff>
--- a/20200506 linux log troubleshooting 特征V4.0.xlsx
+++ b/20200506 linux log troubleshooting 特征V4.0.xlsx
@@ -10,12 +10,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$53</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="102">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,10 +68,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/var/log/messages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/var/log/syslog</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -254,11 +253,6 @@
   </si>
   <si>
     <t>系统磁盘空间告警</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/var/log/secure
-/var/log/auth.log</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -424,6 +418,23 @@
   </si>
   <si>
     <t>zengxl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>warn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/messages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/kernel.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/secure
+/var/log/auth.log</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -860,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -887,7 +898,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -896,7 +907,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
@@ -911,19 +922,19 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -935,7 +946,7 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -944,10 +955,10 @@
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -959,7 +970,7 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -968,7 +979,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -981,16 +992,16 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1003,19 +1014,19 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1027,19 +1038,19 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1051,16 +1062,16 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1073,16 +1084,16 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -1095,16 +1106,16 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -1113,20 +1124,20 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1135,20 +1146,20 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -1157,20 +1168,20 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -1179,20 +1190,20 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -1201,20 +1212,20 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -1224,19 +1235,19 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>92</v>
+        <v>28</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -1246,19 +1257,19 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1268,19 +1279,19 @@
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>92</v>
+        <v>29</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -1290,19 +1301,19 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -1312,19 +1323,19 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -1334,19 +1345,19 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -1356,16 +1367,16 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1376,16 +1387,16 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1396,19 +1407,19 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="33" x14ac:dyDescent="0.3">
@@ -1416,21 +1427,21 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1438,20 +1449,20 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" s="1"/>
     </row>
@@ -1460,20 +1471,20 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H27" s="1"/>
     </row>
@@ -1482,20 +1493,20 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -1504,20 +1515,20 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="G29" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" s="1"/>
     </row>
@@ -1526,20 +1537,20 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" s="1"/>
     </row>
@@ -1548,20 +1559,20 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" s="1"/>
     </row>
@@ -1570,20 +1581,20 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -1592,20 +1603,20 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" s="1"/>
     </row>
@@ -1614,23 +1625,23 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="3" t="s">
-        <v>93</v>
+      <c r="D34" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1638,20 +1649,20 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -1660,20 +1671,20 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H36" s="1"/>
     </row>
@@ -1682,20 +1693,20 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H37" s="1"/>
     </row>
@@ -1704,21 +1715,21 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1726,21 +1737,21 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1748,21 +1759,21 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1770,21 +1781,21 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1792,21 +1803,21 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1814,21 +1825,21 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1836,21 +1847,21 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1858,21 +1869,21 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1880,21 +1891,21 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1902,21 +1913,21 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1924,21 +1935,21 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1946,21 +1957,21 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1968,21 +1979,21 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -1990,21 +2001,21 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -2012,21 +2023,21 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
@@ -2034,21 +2045,21 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F53" s="9" t="s">
-        <v>78</v>
-      </c>
       <c r="G53" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -2137,10 +2148,10 @@
         <v>43960</v>
       </c>
       <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
         <v>96</v>
-      </c>
-      <c r="C1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2148,10 +2159,10 @@
         <v>43962</v>
       </c>
       <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
         <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ceph disk sector log tag
</commit_message>
<xml_diff>
--- a/20200506 linux log troubleshooting 特征V4.0.xlsx
+++ b/20200506 linux log troubleshooting 特征V4.0.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$60</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="109">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -435,6 +435,34 @@
   <si>
     <t>/var/log/secure
 /var/log/auth.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ceph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>print_req_error: critical medium error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/syslog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ubuntu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>硬盘坏扇区故障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>critical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内核 基本日志</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -869,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1119,53 +1147,55 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>82</v>
+        <v>107</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="1"/>
+        <v>108</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="10" t="s">
-        <v>90</v>
+      <c r="D12" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
@@ -1175,29 +1205,29 @@
         <v>90</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="3" t="s">
-        <v>91</v>
+      <c r="D14" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>82</v>
@@ -1209,7 +1239,7 @@
     </row>
     <row r="15" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>23</v>
@@ -1219,41 +1249,41 @@
         <v>91</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>47</v>
+        <v>22</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -1263,10 +1293,10 @@
         <v>91</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>34</v>
@@ -1275,73 +1305,73 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
@@ -1351,39 +1381,41 @@
         <v>91</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
@@ -1393,7 +1425,7 @@
         <v>91</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>77</v>
@@ -1403,7 +1435,7 @@
     </row>
     <row r="24" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
@@ -1413,62 +1445,60 @@
         <v>91</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8" t="s">
+      <c r="B26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F26" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H26" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
@@ -1481,7 +1511,7 @@
         <v>42</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>14</v>
@@ -1490,20 +1520,20 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="3" t="s">
-        <v>91</v>
+      <c r="D28" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>14</v>
@@ -1512,7 +1542,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>23</v>
@@ -1525,7 +1555,7 @@
         <v>43</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>14</v>
@@ -1534,7 +1564,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>23</v>
@@ -1547,16 +1577,16 @@
         <v>43</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>23</v>
@@ -1566,10 +1596,10 @@
         <v>91</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>80</v>
+        <v>43</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>14</v>
@@ -1578,7 +1608,7 @@
     </row>
     <row r="32" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>23</v>
@@ -1587,8 +1617,8 @@
       <c r="D32" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>46</v>
+      <c r="E32" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>80</v>
@@ -1600,7 +1630,7 @@
     </row>
     <row r="33" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>23</v>
@@ -1609,66 +1639,66 @@
       <c r="D33" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>54</v>
+      <c r="E33" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="10" t="s">
-        <v>98</v>
+      <c r="D34" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F34" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>23</v>
@@ -1681,7 +1711,7 @@
         <v>57</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>58</v>
@@ -1690,7 +1720,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>23</v>
@@ -1703,38 +1733,38 @@
         <v>57</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>58</v>
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>85</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>23</v>
@@ -1742,7 +1772,7 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>76</v>
@@ -1756,7 +1786,7 @@
     </row>
     <row r="40" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>23</v>
@@ -1764,7 +1794,7 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>76</v>
@@ -1778,7 +1808,7 @@
     </row>
     <row r="41" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>23</v>
@@ -1786,7 +1816,7 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>76</v>
@@ -1800,7 +1830,7 @@
     </row>
     <row r="42" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>23</v>
@@ -1808,7 +1838,7 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>76</v>
@@ -1822,7 +1852,7 @@
     </row>
     <row r="43" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>23</v>
@@ -1830,7 +1860,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>76</v>
@@ -1844,7 +1874,7 @@
     </row>
     <row r="44" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>23</v>
@@ -1852,7 +1882,7 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F44" s="9" t="s">
         <v>76</v>
@@ -1866,7 +1896,7 @@
     </row>
     <row r="45" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>23</v>
@@ -1874,7 +1904,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>76</v>
@@ -1888,7 +1918,7 @@
     </row>
     <row r="46" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>23</v>
@@ -1896,7 +1926,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F46" s="9" t="s">
         <v>76</v>
@@ -1910,7 +1940,7 @@
     </row>
     <row r="47" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>23</v>
@@ -1918,7 +1948,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F47" s="9" t="s">
         <v>76</v>
@@ -1932,7 +1962,7 @@
     </row>
     <row r="48" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>23</v>
@@ -1940,7 +1970,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F48" s="9" t="s">
         <v>76</v>
@@ -1954,7 +1984,7 @@
     </row>
     <row r="49" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>23</v>
@@ -1962,7 +1992,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>76</v>
@@ -1976,7 +2006,7 @@
     </row>
     <row r="50" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>23</v>
@@ -1984,7 +2014,7 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F50" s="9" t="s">
         <v>76</v>
@@ -1998,7 +2028,7 @@
     </row>
     <row r="51" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>23</v>
@@ -2006,7 +2036,7 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F51" s="9" t="s">
         <v>76</v>
@@ -2020,7 +2050,7 @@
     </row>
     <row r="52" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>23</v>
@@ -2028,7 +2058,7 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>76</v>
@@ -2042,7 +2072,7 @@
     </row>
     <row r="53" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>23</v>
@@ -2050,7 +2080,7 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>76</v>
@@ -2062,24 +2092,46 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+    <row r="54" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -2122,7 +2174,18 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+    </row>
   </sheetData>
+  <autoFilter ref="E1:E60"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>